<commit_message>
I made it so that the user's questions could be understood.
</commit_message>
<xml_diff>
--- a/conversatie.xlsx
+++ b/conversatie.xlsx
@@ -448,72 +448,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Bot</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alexandru</t>
+          <t>Salut! Cum te numești?</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bot</t>
+          <t>User</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cu ce te ocupi?</t>
+          <t>ma numesc Alexandru</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Bot</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Programare</t>
+          <t>Sunt un asistent virtual simplu.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bot</t>
+          <t>User</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ce te interesează cel mai mult acum?</t>
+          <t>ce faci?</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>User</t>
+          <t>Bot</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Python</t>
+          <t>Sunt bine, mulțumesc că întrebi!</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bot</t>
+          <t>User</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Îți mulțumesc, Alexandru! E grozav că ești implicat în Programare și te interesează Python. Sper să-ți fiu de folos!</t>
+          <t>ce poti zice despre python?</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Conversatia a fost incheiata. Mulțumesc!</t>
+          <t>Sunt un asistent virtual simplu.</t>
         </is>
       </c>
     </row>

</xml_diff>